<commit_message>
automation assignment corejava module 6 updated
</commit_message>
<xml_diff>
--- a/MANUAL/PROJECT/HLR PROJECT.xlsx
+++ b/MANUAL/PROJECT/HLR PROJECT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashh\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TESTING\MANUAL\PROJECT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="92">
   <si>
     <t>project name</t>
   </si>
@@ -38,13 +38,7 @@
     <t>xyz</t>
   </si>
   <si>
-    <t>Tester Name</t>
-  </si>
-  <si>
     <t>Raichand.</t>
-  </si>
-  <si>
-    <t>Version</t>
   </si>
   <si>
     <t>Featre No.</t>
@@ -704,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="111" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -724,7 +718,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -814,10 +808,10 @@
     </row>
     <row r="6" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -845,7 +839,7 @@
     </row>
     <row r="7" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C7" s="5">
         <v>1</v>
@@ -876,13 +870,13 @@
     </row>
     <row r="10" spans="1:26" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>7</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
@@ -890,10 +884,10 @@
         <v>1</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
@@ -901,10 +895,10 @@
         <v>2</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
@@ -912,10 +906,10 @@
         <v>3</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
@@ -923,10 +917,10 @@
         <v>4</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
@@ -934,10 +928,10 @@
         <v>5</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
@@ -945,10 +939,10 @@
         <v>6</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -956,10 +950,10 @@
         <v>7</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -967,10 +961,10 @@
         <v>8</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -978,10 +972,10 @@
         <v>9</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -989,10 +983,10 @@
         <v>10</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1000,10 +994,10 @@
         <v>11</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1011,10 +1005,10 @@
         <v>12</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1022,10 +1016,10 @@
         <v>13</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1033,10 +1027,10 @@
         <v>14</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1044,10 +1038,10 @@
         <v>15</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -1055,10 +1049,10 @@
         <v>16</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -1066,10 +1060,10 @@
         <v>17</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -1077,10 +1071,10 @@
         <v>18</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1088,10 +1082,10 @@
         <v>19</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -1099,10 +1093,10 @@
         <v>20</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1110,10 +1104,10 @@
         <v>21</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -1121,10 +1115,10 @@
         <v>22</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -1132,10 +1126,10 @@
         <v>23</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -1143,10 +1137,10 @@
         <v>24</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -1154,10 +1148,10 @@
         <v>25</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1165,10 +1159,10 @@
         <v>26</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1176,10 +1170,10 @@
         <v>27</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1187,10 +1181,10 @@
         <v>28</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1198,10 +1192,10 @@
         <v>29</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1209,10 +1203,10 @@
         <v>30</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1220,10 +1214,10 @@
         <v>31</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1231,10 +1225,10 @@
         <v>32</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1242,10 +1236,10 @@
         <v>33</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -1253,10 +1247,10 @@
         <v>34</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -1264,10 +1258,10 @@
         <v>35</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1275,10 +1269,10 @@
         <v>36</v>
       </c>
       <c r="B46" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -1286,10 +1280,10 @@
         <v>37</v>
       </c>
       <c r="B47" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1297,10 +1291,10 @@
         <v>38</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1308,10 +1302,10 @@
         <v>39</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -1319,10 +1313,10 @@
         <v>40</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1330,10 +1324,10 @@
         <v>41</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1341,10 +1335,10 @@
         <v>42</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>